<commit_message>
Update for popup added
</commit_message>
<xml_diff>
--- a/nurses.xlsx
+++ b/nurses.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -437,9 +437,128 @@
         <v>18</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Daniel</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2147483647</v>
+      </c>
+      <c r="D3" s="1">
+        <v>39008.00011574074</v>
+      </c>
+      <c r="E3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Passion</v>
+      </c>
+      <c r="C4" t="str">
+        <v>1231234324</v>
+      </c>
+      <c r="D4" s="1">
+        <v>39009.00011574074</v>
+      </c>
+      <c r="E4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Kumar</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2147483647</v>
+      </c>
+      <c r="D5" s="1">
+        <v>39008.00011574074</v>
+      </c>
+      <c r="E5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Kamal</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2147483647</v>
+      </c>
+      <c r="D6" s="1">
+        <v>39008.00011574074</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Suresh</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2147483647</v>
+      </c>
+      <c r="D7" s="1">
+        <v>32434.000115740742</v>
+      </c>
+      <c r="E7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="str">
+        <v>qwwerr</v>
+      </c>
+      <c r="C8" t="str">
+        <v>7854551266</v>
+      </c>
+      <c r="D8" s="1">
+        <v>37356.00011574074</v>
+      </c>
+      <c r="E8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="str">
+        <v>ashish</v>
+      </c>
+      <c r="C9" t="str">
+        <v>78955952599</v>
+      </c>
+      <c r="D9" s="1">
+        <v>36642.00011574074</v>
+      </c>
+      <c r="E9">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>